<commit_message>
reorganizing ipynb, added json inputs to dataset import loop.
</commit_message>
<xml_diff>
--- a/test/dataset_index.xlsx
+++ b/test/dataset_index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\Python\ehd_exsitu\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4BD56D-946B-4417-BE6C-C767DEC46001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966634EB-63FD-4E18-8DAD-60879CECE89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6375" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Path</t>
   </si>
@@ -55,12 +55,6 @@
   </si>
   <si>
     <t>harmonics</t>
-  </si>
-  <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>results 2-may-22 run2.xlsx</t>
   </si>
 </sst>
 </file>
@@ -388,63 +382,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="2">
         <v>44683</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="E2">
+      <c r="D2">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="G2">
+      <c r="F2">
         <v>570</v>
       </c>
     </row>

</xml_diff>